<commit_message>
Added the functionality to read excel file
</commit_message>
<xml_diff>
--- a/FirstJavaProj/resources/empExcel.xlsx
+++ b/FirstJavaProj/resources/empExcel.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="empDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,30 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Designation</t>
-  </si>
-  <si>
-    <t>isMgr</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
     <t>Sourav</t>
   </si>
   <si>
-    <t>SDE</t>
-  </si>
-  <si>
     <t>Srikar</t>
   </si>
   <si>
-    <t>Pricipal SD</t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Hi TechCity</t>
+  </si>
+  <si>
+    <t>Madhabpur</t>
   </si>
 </sst>
 </file>
@@ -365,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,23 +375,20 @@
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -401,25 +396,31 @@
       <c r="C2">
         <v>9238392383</v>
       </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>982342235</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>